<commit_message>
Orders for p7 and p8
</commit_message>
<xml_diff>
--- a/editable/Orders/PAR07_RUN01.xlsx
+++ b/editable/Orders/PAR07_RUN01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evade\Documents\GitHub\Zoom_ToM\editable\Orders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelakent/Documents/GitHub/Zoom_ToM/editable/Orders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F28FD7-021B-4B04-A7E2-75A91BDE34CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB34BDAD-87B9-9A4E-9A24-8FF6F27EA8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="396" windowWidth="13824" windowHeight="7176" xr2:uid="{BD61E833-CF50-497D-95A8-C90AF86DCFE3}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="13560" windowHeight="15740" xr2:uid="{BD61E833-CF50-497D-95A8-C90AF86DCFE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Trial</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>ConditionType</t>
+  </si>
+  <si>
+    <t>ITI</t>
   </si>
 </sst>
 </file>
@@ -394,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED83222-3191-4DAB-B718-29CDBE9A9DD3}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +415,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -421,10 +427,13 @@
         <v>37</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -432,10 +441,13 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -443,10 +455,13 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -454,10 +469,13 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -467,8 +485,11 @@
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -476,10 +497,13 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -489,8 +513,11 @@
       <c r="C8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -498,10 +525,13 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -511,8 +541,11 @@
       <c r="C10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -522,8 +555,11 @@
       <c r="C11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -531,10 +567,13 @@
         <v>27</v>
       </c>
       <c r="C12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -542,10 +581,13 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -553,10 +595,13 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -564,10 +609,13 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -575,10 +623,13 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -586,40 +637,10 @@
         <v>23</v>
       </c>
       <c r="C17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>35</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>33</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>